<commit_message>
Closed sprint 7 started sprint 8 added PDF of report for HW3
</commit_message>
<xml_diff>
--- a/project/Sprint07.xlsx
+++ b/project/Sprint07.xlsx
@@ -137,7 +137,8 @@
     <t>HW3 - Home page</t>
   </si>
   <si>
-    <t>Finish HW3 and get paper drafted.</t>
+    <t>Finish HW3 and get paper drafted.
+HW3 took a little longer than anticipated and so paper got pushed back again.</t>
   </si>
 </sst>
 </file>
@@ -531,10 +532,10 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1755,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -1848,11 +1849,11 @@
       </c>
       <c r="J2" s="25">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="K2" s="25">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2100,7 +2101,7 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:K10" si="5">D8</f>
+        <f t="shared" ref="E8:E9" si="5">D8</f>
         <v>3</v>
       </c>
       <c r="F8">
@@ -2204,12 +2205,11 @@
         <v>3</v>
       </c>
       <c r="J10">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2246,12 +2246,11 @@
         <v>3</v>
       </c>
       <c r="J11">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2288,12 +2287,11 @@
         <v>3</v>
       </c>
       <c r="J12">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2314,7 +2312,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F4:K13" si="8">E13</f>
+        <f t="shared" ref="F13:K13" si="8">E13</f>
         <v>1</v>
       </c>
       <c r="G13">
@@ -2330,12 +2328,11 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>